<commit_message>
Task Management System Update
</commit_message>
<xml_diff>
--- a/Task/Task Management System.xlsx
+++ b/Task/Task Management System.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TestCase" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="106">
   <si>
     <t>Product Name</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Developed By</t>
   </si>
   <si>
-    <t>Rabanni</t>
+    <t>Faishel Rabbani</t>
   </si>
   <si>
     <t>Test Case Developed By</t>
@@ -342,9 +342,13 @@
     <t>Should be same Header whole website</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Goto the URL http://niprojmi.com/ 
+    <t>Click</t>
+  </si>
+  <si>
+    <t>1. Goto the URL http://niprojmi.com/ 
 2. Click on Login button 
-3. Click all Button </t>
+3. After Login go to Dashboad
+4. Show all page header</t>
   </si>
   <si>
     <t>Click Dashboard Button</t>
@@ -353,19 +357,123 @@
     <t>Go to dashboard Page</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Goto the URL http://niprojmi.com/ 
+    <t xml:space="preserve">1. Dashboard
+2. Click Dashboard Button </t>
+  </si>
+  <si>
+    <t>Click Reports Button</t>
+  </si>
+  <si>
+    <t>Open All Report Button under Reports button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dashboard
+2.  Click Reports Button </t>
+  </si>
+  <si>
+    <t>Click All Report Button</t>
+  </si>
+  <si>
+    <t>Open A new page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dashboard
+2.  Click All Report Button </t>
+  </si>
+  <si>
+    <t>Click Add SBU</t>
+  </si>
+  <si>
+    <t>Open a new page and open SBU Name add page</t>
+  </si>
+  <si>
+    <t>1. Dashboard
+2. . Click All Report Button</t>
+  </si>
+  <si>
+    <t>Input SBU name</t>
+  </si>
+  <si>
+    <t>Should add SBU</t>
+  </si>
+  <si>
+    <t>ADD SBU</t>
+  </si>
+  <si>
+    <t>1. Dashboard
+2. Add New SBU</t>
+  </si>
+  <si>
+    <t>Click Task Section</t>
+  </si>
+  <si>
+    <t>Open Add and All List Button under Task Section</t>
+  </si>
+  <si>
+    <t>1. Dashboard
+2. Click Task Section</t>
+  </si>
+  <si>
+    <t>In Task Section Click Add</t>
+  </si>
+  <si>
+    <t>Open a new page and open a from add new task</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>1. Dashboard
+2. Click Task Section
+3. Add</t>
+  </si>
+  <si>
+    <t>In Task Section All List</t>
+  </si>
+  <si>
+    <t>Open a new page and show All Task List</t>
+  </si>
+  <si>
+    <t>ALL List</t>
+  </si>
+  <si>
+    <t>1. Dashboard
+2. Click Task Section
+3. All List</t>
+  </si>
+  <si>
+    <t>Verify the same footer used on whole website pages.</t>
+  </si>
+  <si>
+    <t>Should be same Footer whole website</t>
+  </si>
+  <si>
+    <t>1. Goto the URL http://niprojmi.com/ 
 2. Click on Login button 
-3. Click Dashboard Button </t>
-  </si>
-  <si>
-    <t>Click Reports Button</t>
+3. After Login go to Dashboad
+4. Show all page footer</t>
+  </si>
+  <si>
+    <t>Verify the same sideber used on whole website pages</t>
+  </si>
+  <si>
+    <t>Should be same Sideber whole website</t>
+  </si>
+  <si>
+    <t>1. Goto the URL http://niprojmi.com/ 
+2. Click on Login button 
+3. After Login go to Dashboad
+4. Show all page Sideber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -374,7 +482,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
@@ -382,12 +490,12 @@
     <font>
       <b/>
       <u/>
-      <sz val="12.0"/>
+      <sz val="14.0"/>
       <color rgb="FF0563C1"/>
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
@@ -397,18 +505,20 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="10.0"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Verdana"/>
     </font>
     <font>
+      <u/>
+      <sz val="14.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12.0"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="14.0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -444,6 +554,17 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
       <u/>
       <sz val="12.0"/>
       <color rgb="FF0000FF"/>
@@ -459,6 +580,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12.0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Times New Roman&quot;"/>
     </font>
   </fonts>
   <fills count="15">
@@ -730,7 +862,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -746,22 +878,22 @@
     <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="6" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -770,11 +902,11 @@
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="6" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -785,7 +917,7 @@
     <xf borderId="6" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -845,103 +977,115 @@
     <xf borderId="14" fillId="13" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="12" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="12" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="11" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="14" fillId="11" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="11" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="12" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="18" fillId="12" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="14" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="14" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="11" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="19" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1170,12 +1314,12 @@
     <col customWidth="1" min="1" max="1" width="6.86"/>
     <col customWidth="1" min="2" max="2" width="12.29"/>
     <col customWidth="1" min="3" max="3" width="33.0"/>
-    <col customWidth="1" min="4" max="4" width="22.14"/>
-    <col customWidth="1" min="5" max="5" width="21.86"/>
+    <col customWidth="1" min="4" max="4" width="27.86"/>
+    <col customWidth="1" min="5" max="5" width="27.71"/>
     <col customWidth="1" min="6" max="6" width="25.43"/>
     <col customWidth="1" min="7" max="7" width="30.86"/>
     <col customWidth="1" min="8" max="8" width="31.29"/>
-    <col customWidth="1" min="9" max="9" width="20.57"/>
+    <col customWidth="1" min="9" max="9" width="25.14"/>
     <col customWidth="1" min="10" max="10" width="15.14"/>
     <col customWidth="1" min="11" max="11" width="15.57"/>
     <col customWidth="1" min="12" max="12" width="14.71"/>
@@ -1194,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="5">
-        <v>45203.0</v>
+        <v>45026.0</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>3</v>
@@ -1212,13 +1356,13 @@
       <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="8"/>
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="10">
         <f>COUNTIF(K8:K157,"Passed")</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="27.0" customHeight="1">
@@ -1267,7 +1411,7 @@
       </c>
       <c r="L6" s="20">
         <f>SUM(L2:L5)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
@@ -1626,9 +1770,7 @@
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
       <c r="J19" s="63"/>
-      <c r="K19" s="64" t="s">
-        <v>34</v>
-      </c>
+      <c r="K19" s="64"/>
       <c r="L19" s="63"/>
       <c r="M19" s="65"/>
       <c r="N19" s="65"/>
@@ -1646,12 +1788,12 @@
       <c r="Z19" s="65"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="66">
+      <c r="A20" s="56">
         <f>sum(10+1)</f>
         <v>11</v>
       </c>
       <c r="B20" s="39"/>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="66" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="40"/>
@@ -1664,11 +1806,11 @@
       <c r="G20" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="57" t="s">
-        <v>39</v>
+      <c r="H20" s="67" t="s">
+        <v>71</v>
       </c>
       <c r="I20" s="57" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J20" s="59"/>
       <c r="K20" s="55" t="s">
@@ -1677,27 +1819,27 @@
       <c r="L20" s="59"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="66">
+      <c r="A21" s="56">
         <f t="shared" ref="A21:A33" si="2">sum(A20+1)</f>
         <v>12</v>
       </c>
       <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="40"/>
       <c r="E21" s="57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="57" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G21" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H21" s="57" t="s">
-        <v>39</v>
+      <c r="H21" s="67" t="s">
+        <v>71</v>
       </c>
       <c r="I21" s="57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J21" s="59"/>
       <c r="K21" s="55" t="s">
@@ -1706,22 +1848,28 @@
       <c r="L21" s="59"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="66">
+      <c r="A22" s="56">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="40"/>
       <c r="E22" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="59"/>
+        <v>76</v>
+      </c>
+      <c r="F22" s="57" t="s">
+        <v>77</v>
+      </c>
       <c r="G22" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
+      <c r="H22" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="57" t="s">
+        <v>78</v>
+      </c>
       <c r="J22" s="59"/>
       <c r="K22" s="55" t="s">
         <v>34</v>
@@ -1729,20 +1877,28 @@
       <c r="L22" s="59"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="66">
+      <c r="A23" s="56">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
+      <c r="E23" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="57" t="s">
+        <v>80</v>
+      </c>
       <c r="G23" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
+      <c r="H23" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="57" t="s">
+        <v>81</v>
+      </c>
       <c r="J23" s="59"/>
       <c r="K23" s="55" t="s">
         <v>34</v>
@@ -1750,20 +1906,28 @@
       <c r="L23" s="59"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="66">
+      <c r="A24" s="56">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="B24" s="39"/>
-      <c r="C24" s="40"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
+      <c r="E24" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>83</v>
+      </c>
       <c r="G24" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
+      <c r="H24" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="69" t="s">
+        <v>84</v>
+      </c>
       <c r="J24" s="59"/>
       <c r="K24" s="55" t="s">
         <v>34</v>
@@ -1771,20 +1935,28 @@
       <c r="L24" s="59"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="66">
+      <c r="A25" s="56">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
+      <c r="C25" s="45"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="E25" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="57" t="s">
+        <v>86</v>
+      </c>
       <c r="G25" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
+      <c r="H25" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="57" t="s">
+        <v>88</v>
+      </c>
       <c r="J25" s="59"/>
       <c r="K25" s="55" t="s">
         <v>34</v>
@@ -1792,20 +1964,28 @@
       <c r="L25" s="59"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="66">
+      <c r="A26" s="56">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="B26" s="39"/>
-      <c r="C26" s="40"/>
+      <c r="C26" s="45"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
+      <c r="E26" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="57" t="s">
+        <v>90</v>
+      </c>
       <c r="G26" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
+      <c r="H26" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="57" t="s">
+        <v>91</v>
+      </c>
       <c r="J26" s="59"/>
       <c r="K26" s="55" t="s">
         <v>34</v>
@@ -1813,20 +1993,28 @@
       <c r="L26" s="59"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="66">
+      <c r="A27" s="56">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="B27" s="39"/>
-      <c r="C27" s="40"/>
+      <c r="C27" s="45"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
+      <c r="E27" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>93</v>
+      </c>
       <c r="G27" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
+      <c r="H27" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="57" t="s">
+        <v>95</v>
+      </c>
       <c r="J27" s="59"/>
       <c r="K27" s="55" t="s">
         <v>34</v>
@@ -1834,20 +2022,28 @@
       <c r="L27" s="59"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="66">
+      <c r="A28" s="56">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="B28" s="39"/>
-      <c r="C28" s="40"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
+      <c r="E28" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="57" t="s">
+        <v>97</v>
+      </c>
       <c r="G28" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
+      <c r="H28" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" s="57" t="s">
+        <v>99</v>
+      </c>
       <c r="J28" s="59"/>
       <c r="K28" s="55" t="s">
         <v>34</v>
@@ -1855,20 +2051,28 @@
       <c r="L28" s="59"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="66">
+      <c r="A29" s="56">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>101</v>
+      </c>
       <c r="G29" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
+      <c r="H29" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="57" t="s">
+        <v>102</v>
+      </c>
       <c r="J29" s="59"/>
       <c r="K29" s="55" t="s">
         <v>34</v>
@@ -1876,20 +2080,28 @@
       <c r="L29" s="59"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="66">
+      <c r="A30" s="72">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>104</v>
+      </c>
       <c r="G30" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
+      <c r="H30" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="57" t="s">
+        <v>105</v>
+      </c>
       <c r="J30" s="59"/>
       <c r="K30" s="55" t="s">
         <v>34</v>
@@ -1897,19 +2109,19 @@
       <c r="L30" s="59"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="71">
+      <c r="A31" s="75">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="71">
+      <c r="A32" s="75">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="71">
+      <c r="A33" s="75">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -2869,30 +3081,39 @@
     <row r="986" ht="13.5" customHeight="1"/>
     <row r="987" ht="13.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B10:B18"/>
+    <mergeCell ref="C10:C18"/>
     <mergeCell ref="D10:D18"/>
-    <mergeCell ref="C10:C18"/>
-    <mergeCell ref="B10:B18"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="C20:C30"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="K8 K10:K30">
+    <dataValidation type="list" allowBlank="1" sqref="K8 K10:K18 K20:K30">
       <formula1>"Passed,Failed,Not Executed,Out of Scope"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C1"/>
-    <hyperlink r:id="rId2" ref="I8"/>
-    <hyperlink r:id="rId3" ref="I15"/>
-    <hyperlink r:id="rId4" ref="I18"/>
+    <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="E3"/>
+    <hyperlink r:id="rId4" ref="I8"/>
+    <hyperlink r:id="rId5" ref="I15"/>
+    <hyperlink r:id="rId6" ref="I18"/>
+    <hyperlink r:id="rId7" ref="H23"/>
+    <hyperlink r:id="rId8" ref="H24"/>
+    <hyperlink r:id="rId9" ref="H25"/>
+    <hyperlink r:id="rId10" ref="H26"/>
+    <hyperlink r:id="rId11" ref="H27"/>
+    <hyperlink r:id="rId12" ref="H28"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>